<commit_message>
changed more entity values. changed column name in matrix to male:female
</commit_message>
<xml_diff>
--- a/CDSData/CDS_SPARSE_2020_2021.xlsx
+++ b/CDSData/CDS_SPARSE_2020_2021.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhengy6\Desktop\rhit_IRPA_2023\CDSData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kimj16\Documents\497\rhit_IRPA_2023\CDSData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ECCEAD9-78FE-4B35-8941-F0CCAB62A20A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C07E3B9-BA7D-453B-87BC-5D45AF7C3445}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{FE1ED6D0-6606-421C-9DB9-B4886BF13D14}"/>
+    <workbookView xWindow="1500" yWindow="1500" windowWidth="14808" windowHeight="10116" xr2:uid="{FE1ED6D0-6606-421C-9DB9-B4886BF13D14}"/>
   </bookViews>
   <sheets>
     <sheet name="General_Enrollment" sheetId="1" r:id="rId1"/>
@@ -99,12 +99,6 @@
     <t>undergraduate</t>
   </si>
   <si>
-    <t>men</t>
-  </si>
-  <si>
-    <t>women</t>
-  </si>
-  <si>
     <t>Value</t>
   </si>
   <si>
@@ -112,6 +106,12 @@
   </si>
   <si>
     <t>african-american</t>
+  </si>
+  <si>
+    <t>male</t>
+  </si>
+  <si>
+    <t>female</t>
   </si>
 </sst>
 </file>
@@ -465,15 +465,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{224585FE-606B-4F40-9ACE-2F85812D2681}">
   <dimension ref="A1:P41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D49" sqref="D49"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B1" t="s">
         <v>19</v>
@@ -488,10 +488,10 @@
         <v>1</v>
       </c>
       <c r="F1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="G1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="H1" t="s">
         <v>2</v>
@@ -2530,7 +2530,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2EB211C-713F-433C-AADD-E85D0317D8A2}">
   <dimension ref="A1:Q21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
@@ -2554,7 +2554,7 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B1" t="s">
         <v>15</v>
@@ -2563,7 +2563,7 @@
         <v>9</v>
       </c>
       <c r="D1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E1" t="s">
         <v>10</v>
@@ -2578,7 +2578,7 @@
         <v>17</v>
       </c>
       <c r="I1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="J1" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
fixed issue with graduation rate query
</commit_message>
<xml_diff>
--- a/CDSData/CDS_SPARSE_2020_2021.xlsx
+++ b/CDSData/CDS_SPARSE_2020_2021.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhengy6\Desktop\rhit_IRPA_2023\CDSData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kimj16\Documents\497\rhit_IRPA_2023\CDSData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ECCEAD9-78FE-4B35-8941-F0CCAB62A20A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C07E3B9-BA7D-453B-87BC-5D45AF7C3445}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{FE1ED6D0-6606-421C-9DB9-B4886BF13D14}"/>
+    <workbookView xWindow="1500" yWindow="1500" windowWidth="14808" windowHeight="10116" xr2:uid="{FE1ED6D0-6606-421C-9DB9-B4886BF13D14}"/>
   </bookViews>
   <sheets>
     <sheet name="General_Enrollment" sheetId="1" r:id="rId1"/>
@@ -99,12 +99,6 @@
     <t>undergraduate</t>
   </si>
   <si>
-    <t>men</t>
-  </si>
-  <si>
-    <t>women</t>
-  </si>
-  <si>
     <t>Value</t>
   </si>
   <si>
@@ -112,6 +106,12 @@
   </si>
   <si>
     <t>african-american</t>
+  </si>
+  <si>
+    <t>male</t>
+  </si>
+  <si>
+    <t>female</t>
   </si>
 </sst>
 </file>
@@ -465,15 +465,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{224585FE-606B-4F40-9ACE-2F85812D2681}">
   <dimension ref="A1:P41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D49" sqref="D49"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B1" t="s">
         <v>19</v>
@@ -488,10 +488,10 @@
         <v>1</v>
       </c>
       <c r="F1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="G1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="H1" t="s">
         <v>2</v>
@@ -2530,7 +2530,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2EB211C-713F-433C-AADD-E85D0317D8A2}">
   <dimension ref="A1:Q21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
@@ -2554,7 +2554,7 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B1" t="s">
         <v>15</v>
@@ -2563,7 +2563,7 @@
         <v>9</v>
       </c>
       <c r="D1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E1" t="s">
         <v>10</v>
@@ -2578,7 +2578,7 @@
         <v>17</v>
       </c>
       <c r="I1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="J1" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
fixed bug with selecting wrong sparse matrix and created new internal data models for encapsulation
</commit_message>
<xml_diff>
--- a/CDSData/CDS_SPARSE_2020_2021.xlsx
+++ b/CDSData/CDS_SPARSE_2020_2021.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhengy6\Desktop\rhit_IRPA_2023\CDSData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D39C4D2F-BEF3-404B-BACE-8BB153956527}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DE83E6F-F965-46EB-A694-0A806B1ECDBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{FE1ED6D0-6606-421C-9DB9-B4886BF13D14}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FE1ED6D0-6606-421C-9DB9-B4886BF13D14}"/>
   </bookViews>
   <sheets>
     <sheet name="General_Enrollment" sheetId="1" r:id="rId1"/>
-    <sheet name="Enrollment_by_Race" sheetId="2" r:id="rId2"/>
+    <sheet name="Race_Enrollment" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -465,13 +465,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{224585FE-606B-4F40-9ACE-2F85812D2681}">
   <dimension ref="A1:P41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="10.5546875" customWidth="1"/>
+    <col min="11" max="11" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.44140625" customWidth="1"/>
+    <col min="15" max="15" width="15" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.3">
@@ -2533,8 +2536,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2EB211C-713F-433C-AADD-E85D0317D8A2}">
   <dimension ref="A1:Q21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
created high school unit sparse matrix, training data, backend logic and test stories, will have to test this more
</commit_message>
<xml_diff>
--- a/CDSData/CDS_SPARSE_2020_2021.xlsx
+++ b/CDSData/CDS_SPARSE_2020_2021.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhengy6\Desktop\rhit_IRPA_2023\CDSData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{314C0D26-DB73-4E26-846C-BCC354429501}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D35B4F5-0420-44A1-89EF-AE3BEC9964B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10536" yWindow="504" windowWidth="15336" windowHeight="8040" activeTab="2" xr2:uid="{FE1ED6D0-6606-421C-9DB9-B4886BF13D14}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{FE1ED6D0-6606-421C-9DB9-B4886BF13D14}"/>
   </bookViews>
   <sheets>
     <sheet name="General_Enrollment" sheetId="1" r:id="rId1"/>
     <sheet name="Race_Enrollment" sheetId="2" r:id="rId2"/>
-    <sheet name="High_School_Units" sheetId="3" r:id="rId3"/>
+    <sheet name="High_School_Units" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -3739,27 +3739,29 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{730CC96F-1BE5-456B-A223-D1A7FDC98783}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B8EDBC5-1947-42D8-8612-3F660123C619}">
   <dimension ref="A1:N23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.77734375" customWidth="1"/>
-    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.5546875" customWidth="1"/>
-    <col min="6" max="6" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.33203125" customWidth="1"/>
-    <col min="9" max="9" width="22.44140625" customWidth="1"/>
-    <col min="10" max="10" width="25.77734375" customWidth="1"/>
-    <col min="11" max="11" width="23" customWidth="1"/>
-    <col min="13" max="13" width="15.33203125" customWidth="1"/>
-    <col min="14" max="14" width="18.5546875" customWidth="1"/>
+    <col min="2" max="2" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.21875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
@@ -4023,7 +4025,7 @@
         <v>1</v>
       </c>
       <c r="N6" cm="1">
-        <f t="array" aca="1" ref="N6" ca="1">B6:N60</f>
+        <f t="array" aca="1" ref="N6" ca="1">B6:N23</f>
         <v>0</v>
       </c>
     </row>
@@ -4112,7 +4114,7 @@
         <v>1</v>
       </c>
       <c r="N8" cm="1">
-        <f t="array" aca="1" ref="N8" ca="1">B8:N62</f>
+        <f t="array" aca="1" ref="N8" ca="1">B8:N23</f>
         <v>0</v>
       </c>
     </row>
@@ -4201,7 +4203,7 @@
         <v>1</v>
       </c>
       <c r="N10" cm="1">
-        <f t="array" aca="1" ref="N10" ca="1">B10:N64</f>
+        <f t="array" aca="1" ref="N10" ca="1">B10:N23</f>
         <v>0</v>
       </c>
     </row>
@@ -4289,8 +4291,7 @@
       <c r="M12">
         <v>1</v>
       </c>
-      <c r="N12" cm="1">
-        <f t="array" aca="1" ref="N12" ca="1">B12:N66</f>
+      <c r="N12">
         <v>0</v>
       </c>
     </row>
@@ -4379,7 +4380,7 @@
         <v>1</v>
       </c>
       <c r="N14" cm="1">
-        <f t="array" aca="1" ref="N14" ca="1">B14:N68</f>
+        <f t="array" aca="1" ref="N14" ca="1">B14:N23</f>
         <v>0</v>
       </c>
     </row>
@@ -4468,7 +4469,7 @@
         <v>1</v>
       </c>
       <c r="N16" cm="1">
-        <f t="array" aca="1" ref="N16" ca="1">B16:N70</f>
+        <f t="array" aca="1" ref="N16" ca="1">B16:N23</f>
         <v>0</v>
       </c>
     </row>
@@ -4557,7 +4558,7 @@
         <v>1</v>
       </c>
       <c r="N18" cm="1">
-        <f t="array" aca="1" ref="N18" ca="1">B18:N72</f>
+        <f t="array" aca="1" ref="N18" ca="1">B18:N23</f>
         <v>0</v>
       </c>
     </row>
@@ -4646,7 +4647,7 @@
         <v>1</v>
       </c>
       <c r="N20" cm="1">
-        <f t="array" aca="1" ref="N20" ca="1">B20:N74</f>
+        <f t="array" aca="1" ref="N20" ca="1">B20:N23</f>
         <v>0</v>
       </c>
     </row>
@@ -4735,7 +4736,7 @@
         <v>1</v>
       </c>
       <c r="N22" cm="1">
-        <f t="array" aca="1" ref="N22" ca="1">B22:N76</f>
+        <f t="array" aca="1" ref="N22" ca="1">B22:N23</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
half way done admission
</commit_message>
<xml_diff>
--- a/CDSData/CDS_SPARSE_2020_2021.xlsx
+++ b/CDSData/CDS_SPARSE_2020_2021.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\rhit_IRPA_2023\CDSData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EAC48AF-CA70-4192-8327-C859BBA9781B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BD02038-EC46-4E12-9422-433AF459A9C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" firstSheet="1" activeTab="2" xr2:uid="{FE1ED6D0-6606-421C-9DB9-B4886BF13D14}"/>
+    <workbookView xWindow="1470" yWindow="1470" windowWidth="16200" windowHeight="9983" firstSheet="1" activeTab="2" xr2:uid="{FE1ED6D0-6606-421C-9DB9-B4886BF13D14}"/>
   </bookViews>
   <sheets>
     <sheet name="General_Enrollment" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="42">
   <si>
     <t>full-time</t>
   </si>
@@ -158,6 +158,12 @@
   </si>
   <si>
     <t>policy</t>
+  </si>
+  <si>
+    <t>female</t>
+  </si>
+  <si>
+    <t>male</t>
   </si>
 </sst>
 </file>
@@ -3721,7 +3727,7 @@
   <dimension ref="A1:S12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R1" sqref="R1"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3740,10 +3746,10 @@
         <v>4</v>
       </c>
       <c r="E1" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="F1" t="s">
-        <v>20</v>
+        <v>41</v>
       </c>
       <c r="G1" t="s">
         <v>25</v>

</xml_diff>

<commit_message>
fix issue with querying high school unit, not loading sparse matrix and shouldAddRowStrategy error
</commit_message>
<xml_diff>
--- a/CDSData/CDS_SPARSE_2020_2021.xlsx
+++ b/CDSData/CDS_SPARSE_2020_2021.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhengy6\Desktop\rhit_IRPA_2023\CDSData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99A637C4-DB74-41AD-ABE4-57EAD136DB1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A561595C-F713-4445-A123-BC54D467FEC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{FE1ED6D0-6606-421C-9DB9-B4886BF13D14}"/>
   </bookViews>
   <sheets>
     <sheet name="General_Enrollment" sheetId="1" r:id="rId1"/>
     <sheet name="Race_Enrollment" sheetId="2" r:id="rId2"/>
-    <sheet name="High_School_Units" sheetId="5" r:id="rId3"/>
+    <sheet name="High School Units" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -3721,7 +3721,7 @@
   <dimension ref="A1:N23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N15" sqref="N15"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4008,7 +4008,7 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B7">
         <v>0</v>

</xml_diff>

<commit_message>
created response for high school units and fixed training data
</commit_message>
<xml_diff>
--- a/CDSData/CDS_SPARSE_2020_2021.xlsx
+++ b/CDSData/CDS_SPARSE_2020_2021.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhengy6\Desktop\rhit_IRPA_2023\CDSData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A561595C-F713-4445-A123-BC54D467FEC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AA4C764-6E22-42F2-A7CA-39BBE30E4DD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{FE1ED6D0-6606-421C-9DB9-B4886BF13D14}"/>
   </bookViews>
@@ -124,9 +124,6 @@
     <t>science</t>
   </si>
   <si>
-    <t xml:space="preserve">lab </t>
-  </si>
-  <si>
     <t>foreign-language</t>
   </si>
   <si>
@@ -152,6 +149,9 @@
   </si>
   <si>
     <t>social-studies</t>
+  </si>
+  <si>
+    <t>lab</t>
   </si>
 </sst>
 </file>
@@ -3721,7 +3721,7 @@
   <dimension ref="A1:N23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3730,7 +3730,7 @@
     <col min="2" max="2" width="6.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="3.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125" customWidth="1"/>
     <col min="6" max="6" width="14.77734375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="6.5546875" bestFit="1" customWidth="1"/>
@@ -3756,34 +3756,34 @@
         <v>27</v>
       </c>
       <c r="E1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F1" t="s">
         <v>28</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1" t="s">
         <v>29</v>
       </c>
-      <c r="G1" t="s">
-        <v>37</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>30</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>31</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>32</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>33</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>34</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>35</v>
-      </c>
-      <c r="N1" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
finished high school units and test
</commit_message>
<xml_diff>
--- a/CDSData/CDS_SPARSE_2020_2021.xlsx
+++ b/CDSData/CDS_SPARSE_2020_2021.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhengy6\Desktop\rhit_IRPA_2023\CDSData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AA4C764-6E22-42F2-A7CA-39BBE30E4DD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69FB3AF1-7950-4CE7-9793-A8830CFD1E69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{FE1ED6D0-6606-421C-9DB9-B4886BF13D14}"/>
   </bookViews>
@@ -3721,7 +3721,7 @@
   <dimension ref="A1:N23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4014,13 +4014,13 @@
         <v>0</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -4052,7 +4052,7 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -4061,13 +4061,13 @@
         <v>0</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G8">
         <v>0</v>
@@ -4132,15 +4132,15 @@
         <v>0</v>
       </c>
       <c r="M9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N9">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -4155,10 +4155,10 @@
         <v>0</v>
       </c>
       <c r="F10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H10">
         <v>0</v>
@@ -4176,15 +4176,15 @@
         <v>0</v>
       </c>
       <c r="M10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N10">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -4220,10 +4220,10 @@
         <v>0</v>
       </c>
       <c r="M11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N11">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
@@ -4246,10 +4246,10 @@
         <v>0</v>
       </c>
       <c r="G12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I12">
         <v>0</v>
@@ -4264,10 +4264,10 @@
         <v>0</v>
       </c>
       <c r="M12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N12">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
@@ -4308,10 +4308,10 @@
         <v>0</v>
       </c>
       <c r="M13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N13">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
@@ -4352,10 +4352,10 @@
         <v>0</v>
       </c>
       <c r="M14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
@@ -4396,10 +4396,10 @@
         <v>0</v>
       </c>
       <c r="M15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N15">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
@@ -4425,10 +4425,10 @@
         <v>0</v>
       </c>
       <c r="H16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J16">
         <v>0</v>
@@ -4440,10 +4440,10 @@
         <v>0</v>
       </c>
       <c r="M16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N16">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.3">
@@ -4484,15 +4484,15 @@
         <v>0</v>
       </c>
       <c r="M17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N17">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B18">
         <v>0</v>
@@ -4516,10 +4516,10 @@
         <v>0</v>
       </c>
       <c r="I18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K18">
         <v>0</v>
@@ -4528,10 +4528,10 @@
         <v>0</v>
       </c>
       <c r="M18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N18">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.3">
@@ -4572,10 +4572,10 @@
         <v>0</v>
       </c>
       <c r="M19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N19">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.3">
@@ -4607,19 +4607,19 @@
         <v>0</v>
       </c>
       <c r="J20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L20">
         <v>0</v>
       </c>
       <c r="M20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N20">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.3">
@@ -4660,10 +4660,10 @@
         <v>0</v>
       </c>
       <c r="M21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N21">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.3">
@@ -4698,16 +4698,16 @@
         <v>0</v>
       </c>
       <c r="K22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N22">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.3">
@@ -4748,10 +4748,10 @@
         <v>1</v>
       </c>
       <c r="M23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N23">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
debugged merge changes -- seems to work mostly
</commit_message>
<xml_diff>
--- a/CDSData/CDS_SPARSE_2020_2021.xlsx
+++ b/CDSData/CDS_SPARSE_2020_2021.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhengy6\Desktop\rhit_IRPA_2023\CDSData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69FB3AF1-7950-4CE7-9793-A8830CFD1E69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28BD36AD-D19E-4472-BDC9-34933981F435}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{FE1ED6D0-6606-421C-9DB9-B4886BF13D14}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="General_Enrollment" sheetId="1" r:id="rId1"/>
     <sheet name="Race_Enrollment" sheetId="2" r:id="rId2"/>
     <sheet name="High School Units" sheetId="5" r:id="rId3"/>
+    <sheet name="Admission_General" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="54">
   <si>
     <t>full-time</t>
   </si>
@@ -152,6 +153,54 @@
   </si>
   <si>
     <t>lab</t>
+  </si>
+  <si>
+    <t>women</t>
+  </si>
+  <si>
+    <t>men</t>
+  </si>
+  <si>
+    <t>applied</t>
+  </si>
+  <si>
+    <t>admitted</t>
+  </si>
+  <si>
+    <t>enrolled</t>
+  </si>
+  <si>
+    <t>waiting-list-policy</t>
+  </si>
+  <si>
+    <t>offered-list</t>
+  </si>
+  <si>
+    <t>accepted-list</t>
+  </si>
+  <si>
+    <t>admitted-list</t>
+  </si>
+  <si>
+    <t>list-rank</t>
+  </si>
+  <si>
+    <t>completion-requirement</t>
+  </si>
+  <si>
+    <t>college-preparatory-program</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>High school diploma is required and GED is not accepted</t>
+  </si>
+  <si>
+    <t>Require</t>
   </si>
 </sst>
 </file>
@@ -3721,7 +3770,7 @@
   <dimension ref="A1:N23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4014,10 +4063,10 @@
         <v>0</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7">
         <v>0</v>
@@ -4752,6 +4801,821 @@
       </c>
       <c r="N23">
         <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A47D92F9-2667-4F70-8B43-5914DFB5D4D2}">
+  <dimension ref="A1:P16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K1" t="s">
+        <v>44</v>
+      </c>
+      <c r="L1" t="s">
+        <v>45</v>
+      </c>
+      <c r="M1" t="s">
+        <v>46</v>
+      </c>
+      <c r="N1" t="s">
+        <v>47</v>
+      </c>
+      <c r="O1" t="s">
+        <v>48</v>
+      </c>
+      <c r="P1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>3338</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1038</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>2502</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>851</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>401</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>145</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+      <c r="P8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>0</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+      <c r="P9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>50</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>1</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+      <c r="P10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>119</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>1</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>43</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>1</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+      <c r="P12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>14</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <v>1</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <v>0</v>
+      </c>
+      <c r="P13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>51</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <v>0</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
+      <c r="N14">
+        <v>1</v>
+      </c>
+      <c r="O14">
+        <v>0</v>
+      </c>
+      <c r="P14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>52</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <v>0</v>
+      </c>
+      <c r="M15">
+        <v>0</v>
+      </c>
+      <c r="N15">
+        <v>0</v>
+      </c>
+      <c r="O15">
+        <v>1</v>
+      </c>
+      <c r="P15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>53</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <v>0</v>
+      </c>
+      <c r="M16">
+        <v>0</v>
+      </c>
+      <c r="N16">
+        <v>0</v>
+      </c>
+      <c r="O16">
+        <v>0</v>
+      </c>
+      <c r="P16">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
re implemented highschool unit and enrollment by race, and fixed issue with parser to be able to parse sat and act percentile
</commit_message>
<xml_diff>
--- a/CDSData/CDS_SPARSE_2020_2021.xlsx
+++ b/CDSData/CDS_SPARSE_2020_2021.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhengy6\Desktop\rhit_IRPA_2023\CDSData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1EC4691-E382-436F-9E5D-0B3E14429580}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49A1146E-0A32-4725-97E5-BE51F06FFBF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Enrollment_General" sheetId="1" r:id="rId1"/>
@@ -18,13 +18,14 @@
     <sheet name="High School Units" sheetId="3" r:id="rId3"/>
     <sheet name="Admission_General" sheetId="4" r:id="rId4"/>
     <sheet name="Basis For Selection" sheetId="5" r:id="rId5"/>
+    <sheet name="Freshman Profile_percentile" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="112">
   <si>
     <t>Value</t>
   </si>
@@ -258,13 +259,115 @@
   </si>
   <si>
     <t>not considerd</t>
+  </si>
+  <si>
+    <t>act</t>
+  </si>
+  <si>
+    <t>sat</t>
+  </si>
+  <si>
+    <t>percent</t>
+  </si>
+  <si>
+    <t>25th percentile</t>
+  </si>
+  <si>
+    <t>composite</t>
+  </si>
+  <si>
+    <t>reading</t>
+  </si>
+  <si>
+    <t>writing</t>
+  </si>
+  <si>
+    <t>application essay</t>
+  </si>
+  <si>
+    <t>50th percentile</t>
+  </si>
+  <si>
+    <t>75th percentile</t>
+  </si>
+  <si>
+    <t>mean</t>
+  </si>
+  <si>
+    <t>350</t>
+  </si>
+  <si>
+    <t>296</t>
+  </si>
+  <si>
+    <t>65.9%</t>
+  </si>
+  <si>
+    <t>55.7%</t>
+  </si>
+  <si>
+    <t>1270</t>
+  </si>
+  <si>
+    <t>610</t>
+  </si>
+  <si>
+    <t>650</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>1355</t>
+  </si>
+  <si>
+    <t>700</t>
+  </si>
+  <si>
+    <t>1440</t>
+  </si>
+  <si>
+    <t>760</t>
+  </si>
+  <si>
+    <t>1352</t>
+  </si>
+  <si>
+    <t>652</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>31</t>
+  </si>
+  <si>
+    <t>31.5</t>
+  </si>
+  <si>
+    <t>33</t>
+  </si>
+  <si>
+    <t>34</t>
+  </si>
+  <si>
+    <t>35</t>
+  </si>
+  <si>
+    <t>30</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -276,11 +379,17 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -291,7 +400,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -325,11 +434,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -338,6 +462,9 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -657,7 +784,7 @@
   <dimension ref="A1:P41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O14" sqref="O14"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2727,8 +2854,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Q21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N20" sqref="N20"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2857,7 +2984,7 @@
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>226</v>
+        <v>190</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -2963,7 +3090,7 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>104</v>
+        <v>70</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -3069,7 +3196,7 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>93</v>
+        <v>62</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -3175,7 +3302,7 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>1295</v>
+        <v>939</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -3281,7 +3408,7 @@
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -3387,7 +3514,7 @@
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>127</v>
+        <v>91</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -3599,7 +3726,7 @@
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -3705,7 +3832,7 @@
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B19">
         <v>0</v>
@@ -3869,10 +3996,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:N23"/>
+  <dimension ref="A1:N22"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4115,7 +4242,7 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -4151,15 +4278,15 @@
         <v>0</v>
       </c>
       <c r="M6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N6">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -4171,7 +4298,7 @@
         <v>1</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -4195,15 +4322,15 @@
         <v>0</v>
       </c>
       <c r="M7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N7">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -4212,13 +4339,13 @@
         <v>0</v>
       </c>
       <c r="D8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G8">
         <v>0</v>
@@ -4283,15 +4410,15 @@
         <v>0</v>
       </c>
       <c r="M9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -4306,10 +4433,10 @@
         <v>0</v>
       </c>
       <c r="F10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H10">
         <v>0</v>
@@ -4327,15 +4454,15 @@
         <v>0</v>
       </c>
       <c r="M10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N10">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -4371,10 +4498,10 @@
         <v>0</v>
       </c>
       <c r="M11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N11">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
@@ -4397,10 +4524,10 @@
         <v>0</v>
       </c>
       <c r="G12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I12">
         <v>0</v>
@@ -4415,10 +4542,10 @@
         <v>0</v>
       </c>
       <c r="M12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N12">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
@@ -4459,10 +4586,10 @@
         <v>0</v>
       </c>
       <c r="M13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N13">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
@@ -4503,10 +4630,10 @@
         <v>0</v>
       </c>
       <c r="M14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N14">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
@@ -4547,10 +4674,10 @@
         <v>0</v>
       </c>
       <c r="M15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N15">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
@@ -4576,10 +4703,10 @@
         <v>0</v>
       </c>
       <c r="H16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J16">
         <v>0</v>
@@ -4591,15 +4718,15 @@
         <v>0</v>
       </c>
       <c r="M16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N16">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -4635,15 +4762,15 @@
         <v>0</v>
       </c>
       <c r="M17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N17">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B18">
         <v>0</v>
@@ -4667,10 +4794,10 @@
         <v>0</v>
       </c>
       <c r="I18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K18">
         <v>0</v>
@@ -4679,10 +4806,10 @@
         <v>0</v>
       </c>
       <c r="M18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N18">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.3">
@@ -4723,10 +4850,10 @@
         <v>0</v>
       </c>
       <c r="M19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N19">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.3">
@@ -4758,19 +4885,19 @@
         <v>0</v>
       </c>
       <c r="J20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L20">
         <v>0</v>
       </c>
       <c r="M20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N20">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.3">
@@ -4811,10 +4938,10 @@
         <v>0</v>
       </c>
       <c r="M21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N21">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.3">
@@ -4849,59 +4976,15 @@
         <v>0</v>
       </c>
       <c r="K22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A23">
-        <v>0</v>
-      </c>
-      <c r="B23">
-        <v>0</v>
-      </c>
-      <c r="C23">
-        <v>0</v>
-      </c>
-      <c r="D23">
-        <v>0</v>
-      </c>
-      <c r="E23">
-        <v>0</v>
-      </c>
-      <c r="F23">
-        <v>0</v>
-      </c>
-      <c r="G23">
-        <v>0</v>
-      </c>
-      <c r="H23">
-        <v>0</v>
-      </c>
-      <c r="I23">
-        <v>0</v>
-      </c>
-      <c r="J23">
-        <v>0</v>
-      </c>
-      <c r="K23">
-        <v>0</v>
-      </c>
-      <c r="L23">
-        <v>1</v>
-      </c>
-      <c r="M23">
-        <v>1</v>
-      </c>
-      <c r="N23">
         <v>0</v>
       </c>
     </row>
@@ -4914,7 +4997,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:P16"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L24" sqref="L24"/>
     </sheetView>
   </sheetViews>
@@ -5733,7 +5816,7 @@
   <dimension ref="A1:T20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7004,4 +7087,1647 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:N37"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O23" sqref="O23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>91</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>93</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>94</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>95</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>96</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>1</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>97</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>1</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>95</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>1</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>98</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>1</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>1</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>96</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>1</v>
+      </c>
+      <c r="K13">
+        <v>1</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>99</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <v>1</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>98</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="H15">
+        <v>1</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <v>1</v>
+      </c>
+      <c r="M15">
+        <v>0</v>
+      </c>
+      <c r="N15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>100</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>1</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <v>1</v>
+      </c>
+      <c r="M16">
+        <v>0</v>
+      </c>
+      <c r="N16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>101</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <v>1</v>
+      </c>
+      <c r="K17">
+        <v>0</v>
+      </c>
+      <c r="L17">
+        <v>1</v>
+      </c>
+      <c r="M17">
+        <v>0</v>
+      </c>
+      <c r="N17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>101</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="L18">
+        <v>0</v>
+      </c>
+      <c r="M18">
+        <v>1</v>
+      </c>
+      <c r="N18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>102</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>1</v>
+      </c>
+      <c r="H19">
+        <v>1</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
+      </c>
+      <c r="K19">
+        <v>0</v>
+      </c>
+      <c r="L19">
+        <v>0</v>
+      </c>
+      <c r="M19">
+        <v>1</v>
+      </c>
+      <c r="N19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>98</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <v>1</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+      <c r="K20">
+        <v>0</v>
+      </c>
+      <c r="L20">
+        <v>0</v>
+      </c>
+      <c r="M20">
+        <v>1</v>
+      </c>
+      <c r="N20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>96</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <v>1</v>
+      </c>
+      <c r="K21">
+        <v>0</v>
+      </c>
+      <c r="L21">
+        <v>0</v>
+      </c>
+      <c r="M21">
+        <v>1</v>
+      </c>
+      <c r="N21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>103</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <v>0</v>
+      </c>
+      <c r="K22">
+        <v>0</v>
+      </c>
+      <c r="L22">
+        <v>0</v>
+      </c>
+      <c r="M22">
+        <v>0</v>
+      </c>
+      <c r="N22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>104</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <v>1</v>
+      </c>
+      <c r="J23">
+        <v>0</v>
+      </c>
+      <c r="K23">
+        <v>0</v>
+      </c>
+      <c r="L23">
+        <v>0</v>
+      </c>
+      <c r="M23">
+        <v>0</v>
+      </c>
+      <c r="N23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>105</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <v>0</v>
+      </c>
+      <c r="J24">
+        <v>0</v>
+      </c>
+      <c r="K24">
+        <v>0</v>
+      </c>
+      <c r="L24">
+        <v>0</v>
+      </c>
+      <c r="M24">
+        <v>0</v>
+      </c>
+      <c r="N24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>96</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <v>1</v>
+      </c>
+      <c r="I25">
+        <v>0</v>
+      </c>
+      <c r="J25">
+        <v>0</v>
+      </c>
+      <c r="K25">
+        <v>0</v>
+      </c>
+      <c r="L25">
+        <v>0</v>
+      </c>
+      <c r="M25">
+        <v>0</v>
+      </c>
+      <c r="N25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>106</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <v>1</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+      <c r="I26">
+        <v>0</v>
+      </c>
+      <c r="J26">
+        <v>0</v>
+      </c>
+      <c r="K26">
+        <v>1</v>
+      </c>
+      <c r="L26">
+        <v>0</v>
+      </c>
+      <c r="M26">
+        <v>0</v>
+      </c>
+      <c r="N26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>106</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27">
+        <v>1</v>
+      </c>
+      <c r="J27">
+        <v>0</v>
+      </c>
+      <c r="K27">
+        <v>1</v>
+      </c>
+      <c r="L27">
+        <v>0</v>
+      </c>
+      <c r="M27">
+        <v>0</v>
+      </c>
+      <c r="N27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>107</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
+      </c>
+      <c r="G28">
+        <v>0</v>
+      </c>
+      <c r="H28">
+        <v>0</v>
+      </c>
+      <c r="I28">
+        <v>0</v>
+      </c>
+      <c r="J28">
+        <v>0</v>
+      </c>
+      <c r="K28">
+        <v>1</v>
+      </c>
+      <c r="L28">
+        <v>0</v>
+      </c>
+      <c r="M28">
+        <v>0</v>
+      </c>
+      <c r="N28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>96</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29">
+        <v>0</v>
+      </c>
+      <c r="G29">
+        <v>0</v>
+      </c>
+      <c r="H29">
+        <v>1</v>
+      </c>
+      <c r="I29">
+        <v>0</v>
+      </c>
+      <c r="J29">
+        <v>0</v>
+      </c>
+      <c r="K29">
+        <v>1</v>
+      </c>
+      <c r="L29">
+        <v>0</v>
+      </c>
+      <c r="M29">
+        <v>0</v>
+      </c>
+      <c r="N29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>108</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30">
+        <v>1</v>
+      </c>
+      <c r="G30">
+        <v>0</v>
+      </c>
+      <c r="H30">
+        <v>0</v>
+      </c>
+      <c r="I30">
+        <v>0</v>
+      </c>
+      <c r="J30">
+        <v>0</v>
+      </c>
+      <c r="K30">
+        <v>0</v>
+      </c>
+      <c r="L30">
+        <v>1</v>
+      </c>
+      <c r="M30">
+        <v>0</v>
+      </c>
+      <c r="N30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>109</v>
+      </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+      <c r="G31">
+        <v>0</v>
+      </c>
+      <c r="H31">
+        <v>0</v>
+      </c>
+      <c r="I31">
+        <v>1</v>
+      </c>
+      <c r="J31">
+        <v>0</v>
+      </c>
+      <c r="K31">
+        <v>0</v>
+      </c>
+      <c r="L31">
+        <v>1</v>
+      </c>
+      <c r="M31">
+        <v>0</v>
+      </c>
+      <c r="N31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>110</v>
+      </c>
+      <c r="B32">
+        <v>1</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="F32">
+        <v>0</v>
+      </c>
+      <c r="G32">
+        <v>0</v>
+      </c>
+      <c r="H32">
+        <v>0</v>
+      </c>
+      <c r="I32">
+        <v>0</v>
+      </c>
+      <c r="J32">
+        <v>0</v>
+      </c>
+      <c r="K32">
+        <v>0</v>
+      </c>
+      <c r="L32">
+        <v>1</v>
+      </c>
+      <c r="M32">
+        <v>0</v>
+      </c>
+      <c r="N32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>96</v>
+      </c>
+      <c r="B33">
+        <v>1</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+      <c r="F33">
+        <v>0</v>
+      </c>
+      <c r="G33">
+        <v>0</v>
+      </c>
+      <c r="H33">
+        <v>1</v>
+      </c>
+      <c r="I33">
+        <v>0</v>
+      </c>
+      <c r="J33">
+        <v>0</v>
+      </c>
+      <c r="K33">
+        <v>0</v>
+      </c>
+      <c r="L33">
+        <v>1</v>
+      </c>
+      <c r="M33">
+        <v>0</v>
+      </c>
+      <c r="N33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>111</v>
+      </c>
+      <c r="B34">
+        <v>1</v>
+      </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="E34">
+        <v>0</v>
+      </c>
+      <c r="F34">
+        <v>1</v>
+      </c>
+      <c r="G34">
+        <v>0</v>
+      </c>
+      <c r="H34">
+        <v>0</v>
+      </c>
+      <c r="I34">
+        <v>0</v>
+      </c>
+      <c r="J34">
+        <v>0</v>
+      </c>
+      <c r="K34">
+        <v>0</v>
+      </c>
+      <c r="L34">
+        <v>0</v>
+      </c>
+      <c r="M34">
+        <v>1</v>
+      </c>
+      <c r="N34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>111</v>
+      </c>
+      <c r="B35">
+        <v>1</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
+      <c r="F35">
+        <v>0</v>
+      </c>
+      <c r="G35">
+        <v>0</v>
+      </c>
+      <c r="H35">
+        <v>0</v>
+      </c>
+      <c r="I35">
+        <v>0</v>
+      </c>
+      <c r="J35">
+        <v>0</v>
+      </c>
+      <c r="K35">
+        <v>0</v>
+      </c>
+      <c r="L35">
+        <v>0</v>
+      </c>
+      <c r="M35">
+        <v>1</v>
+      </c>
+      <c r="N35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>111</v>
+      </c>
+      <c r="B36">
+        <v>1</v>
+      </c>
+      <c r="C36">
+        <v>0</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+      <c r="E36">
+        <v>0</v>
+      </c>
+      <c r="F36">
+        <v>0</v>
+      </c>
+      <c r="G36">
+        <v>0</v>
+      </c>
+      <c r="H36">
+        <v>0</v>
+      </c>
+      <c r="I36">
+        <v>1</v>
+      </c>
+      <c r="J36">
+        <v>0</v>
+      </c>
+      <c r="K36">
+        <v>0</v>
+      </c>
+      <c r="L36">
+        <v>0</v>
+      </c>
+      <c r="M36">
+        <v>1</v>
+      </c>
+      <c r="N36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>96</v>
+      </c>
+      <c r="B37">
+        <v>1</v>
+      </c>
+      <c r="C37">
+        <v>0</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="E37">
+        <v>0</v>
+      </c>
+      <c r="F37">
+        <v>0</v>
+      </c>
+      <c r="G37">
+        <v>0</v>
+      </c>
+      <c r="H37">
+        <v>1</v>
+      </c>
+      <c r="I37">
+        <v>0</v>
+      </c>
+      <c r="J37">
+        <v>0</v>
+      </c>
+      <c r="K37">
+        <v>0</v>
+      </c>
+      <c r="L37">
+        <v>0</v>
+      </c>
+      <c r="M37">
+        <v>1</v>
+      </c>
+      <c r="N37">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
finished freshman profile, added function to determine search result data type
</commit_message>
<xml_diff>
--- a/CDSData/CDS_SPARSE_2020_2021.xlsx
+++ b/CDSData/CDS_SPARSE_2020_2021.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhengy6\Desktop\rhit_IRPA_2023\CDSData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49A1146E-0A32-4725-97E5-BE51F06FFBF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B76763C7-C676-4F6D-A0C8-3AD4219333DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Enrollment_General" sheetId="1" r:id="rId1"/>
@@ -783,16 +783,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="10.5546875" customWidth="1"/>
-    <col min="11" max="11" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.44140625" customWidth="1"/>
-    <col min="15" max="15" width="15" customWidth="1"/>
+    <col min="11" max="11" width="15.44140625" customWidth="1"/>
+    <col min="13" max="13" width="13.88671875" customWidth="1"/>
+    <col min="14" max="14" width="13" customWidth="1"/>
+    <col min="15" max="15" width="15.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.3">
@@ -1089,7 +1089,7 @@
         <v>0</v>
       </c>
       <c r="O6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P6">
         <v>0</v>
@@ -1139,7 +1139,7 @@
         <v>0</v>
       </c>
       <c r="O7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P7">
         <v>0</v>
@@ -1189,7 +1189,7 @@
         <v>0</v>
       </c>
       <c r="O8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P8">
         <v>0</v>
@@ -1239,7 +1239,7 @@
         <v>0</v>
       </c>
       <c r="O9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P9">
         <v>0</v>
@@ -4998,12 +4998,14 @@
   <dimension ref="A1:P16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L24" sqref="L24"/>
+      <selection activeCell="P11" sqref="P11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="21.6640625" customWidth="1"/>
     <col min="10" max="10" width="14.6640625" customWidth="1"/>
+    <col min="16" max="16" width="15" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.3">
@@ -7093,11 +7095,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:N37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O23" sqref="O23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K28" sqref="K28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.77734375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.88671875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">

</xml_diff>

<commit_message>
added training data and defined entities for transfer admission and redesigned entity for high school units need to rewrite test for that
</commit_message>
<xml_diff>
--- a/CDSData/CDS_SPARSE_2020_2021.xlsx
+++ b/CDSData/CDS_SPARSE_2020_2021.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhengy6\Desktop\rhit_IRPA_2023\CDSData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B76763C7-C676-4F6D-A0C8-3AD4219333DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC100C27-42DB-4D11-B003-6A4986DA52EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Enrollment_General" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="113">
   <si>
     <t>Value</t>
   </si>
@@ -135,12 +135,6 @@
     <t>others</t>
   </si>
   <si>
-    <t>units-required</t>
-  </si>
-  <si>
-    <t>units-recommended</t>
-  </si>
-  <si>
     <t>women</t>
   </si>
   <si>
@@ -361,6 +355,15 @@
   </si>
   <si>
     <t>30</t>
+  </si>
+  <si>
+    <t>units</t>
+  </si>
+  <si>
+    <t>require</t>
+  </si>
+  <si>
+    <t>recommend</t>
   </si>
 </sst>
 </file>
@@ -783,7 +786,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
@@ -3996,10 +3999,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:N22"/>
+  <dimension ref="A1:O22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="N25" sqref="N25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4018,9 +4021,10 @@
     <col min="12" max="12" width="6.21875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4058,13 +4062,16 @@
         <v>35</v>
       </c>
       <c r="M1" t="s">
-        <v>36</v>
+        <v>110</v>
       </c>
       <c r="N1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+        <v>111</v>
+      </c>
+      <c r="O1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>4</v>
       </c>
@@ -4105,10 +4112,13 @@
         <v>1</v>
       </c>
       <c r="N2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>0</v>
       </c>
@@ -4146,13 +4156,16 @@
         <v>0</v>
       </c>
       <c r="M3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>4</v>
       </c>
@@ -4193,10 +4206,13 @@
         <v>1</v>
       </c>
       <c r="N4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>5</v>
       </c>
@@ -4234,13 +4250,16 @@
         <v>0</v>
       </c>
       <c r="M5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -4278,13 +4297,16 @@
         <v>0</v>
       </c>
       <c r="M6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>3</v>
       </c>
@@ -4325,10 +4347,13 @@
         <v>1</v>
       </c>
       <c r="N7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>0</v>
       </c>
@@ -4369,10 +4394,13 @@
         <v>1</v>
       </c>
       <c r="N8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>0</v>
       </c>
@@ -4410,13 +4438,16 @@
         <v>0</v>
       </c>
       <c r="M9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>2</v>
       </c>
@@ -4457,10 +4488,13 @@
         <v>1</v>
       </c>
       <c r="N10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>0</v>
       </c>
@@ -4498,13 +4532,16 @@
         <v>0</v>
       </c>
       <c r="M11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>0</v>
       </c>
@@ -4545,10 +4582,13 @@
         <v>1</v>
       </c>
       <c r="N12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>0</v>
       </c>
@@ -4586,13 +4626,16 @@
         <v>0</v>
       </c>
       <c r="M13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>0</v>
       </c>
@@ -4633,10 +4676,13 @@
         <v>1</v>
       </c>
       <c r="N14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="O14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>0</v>
       </c>
@@ -4674,13 +4720,16 @@
         <v>0</v>
       </c>
       <c r="M15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="O15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>0</v>
       </c>
@@ -4721,10 +4770,13 @@
         <v>1</v>
       </c>
       <c r="N16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="O16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>4</v>
       </c>
@@ -4762,13 +4814,16 @@
         <v>0</v>
       </c>
       <c r="M17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="O17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>0</v>
       </c>
@@ -4809,10 +4864,13 @@
         <v>1</v>
       </c>
       <c r="N18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="O18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>0</v>
       </c>
@@ -4850,13 +4908,16 @@
         <v>0</v>
       </c>
       <c r="M19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="O19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>0</v>
       </c>
@@ -4897,10 +4958,13 @@
         <v>1</v>
       </c>
       <c r="N20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="O20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>0</v>
       </c>
@@ -4938,13 +5002,16 @@
         <v>0</v>
       </c>
       <c r="M21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="O21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>0</v>
       </c>
@@ -4985,6 +5052,9 @@
         <v>1</v>
       </c>
       <c r="N22">
+        <v>1</v>
+      </c>
+      <c r="O22">
         <v>0</v>
       </c>
     </row>
@@ -5016,19 +5086,19 @@
         <v>9</v>
       </c>
       <c r="C1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" t="s">
         <v>38</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>39</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>40</v>
-      </c>
-      <c r="F1" t="s">
-        <v>41</v>
-      </c>
-      <c r="G1" t="s">
-        <v>42</v>
       </c>
       <c r="H1" t="s">
         <v>3</v>
@@ -5037,25 +5107,25 @@
         <v>4</v>
       </c>
       <c r="J1" t="s">
+        <v>41</v>
+      </c>
+      <c r="K1" t="s">
+        <v>42</v>
+      </c>
+      <c r="L1" t="s">
         <v>43</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>44</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>45</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>46</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>47</v>
-      </c>
-      <c r="O1" t="s">
-        <v>48</v>
-      </c>
-      <c r="P1" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.3">
@@ -5460,7 +5530,7 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -5660,7 +5730,7 @@
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -5710,7 +5780,7 @@
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -5760,7 +5830,7 @@
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -5850,66 +5920,66 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="O1" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="Q1" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>70</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -5971,7 +6041,7 @@
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -6033,7 +6103,7 @@
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -6095,7 +6165,7 @@
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -6157,7 +6227,7 @@
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -6219,7 +6289,7 @@
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -6281,7 +6351,7 @@
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -6343,7 +6413,7 @@
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -6405,7 +6475,7 @@
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -6467,7 +6537,7 @@
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -6529,7 +6599,7 @@
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -6591,7 +6661,7 @@
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -6653,7 +6723,7 @@
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -6715,7 +6785,7 @@
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -6777,7 +6847,7 @@
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -6839,7 +6909,7 @@
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -6901,7 +6971,7 @@
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B18">
         <v>0</v>
@@ -6963,7 +7033,7 @@
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B19">
         <v>0</v>
@@ -7025,7 +7095,7 @@
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B20">
         <v>0</v>
@@ -7121,40 +7191,40 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>82</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>84</v>
       </c>
       <c r="I1" s="4" t="s">
         <v>26</v>
       </c>
       <c r="J1" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="L1" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>86</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>88</v>
       </c>
       <c r="N1" s="4" t="s">
         <v>25</v>
@@ -7162,7 +7232,7 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -7206,7 +7276,7 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -7250,7 +7320,7 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -7294,7 +7364,7 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -7338,7 +7408,7 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -7382,7 +7452,7 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -7426,7 +7496,7 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -7470,7 +7540,7 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -7514,7 +7584,7 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -7558,7 +7628,7 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -7602,7 +7672,7 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -7646,7 +7716,7 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -7690,7 +7760,7 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -7734,7 +7804,7 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -7778,7 +7848,7 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -7822,7 +7892,7 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -7866,7 +7936,7 @@
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B18">
         <v>0</v>
@@ -7910,7 +7980,7 @@
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B19">
         <v>0</v>
@@ -7954,7 +8024,7 @@
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B20">
         <v>0</v>
@@ -7998,7 +8068,7 @@
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B21">
         <v>0</v>
@@ -8042,7 +8112,7 @@
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -8086,7 +8156,7 @@
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -8130,7 +8200,7 @@
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -8174,7 +8244,7 @@
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B25">
         <v>1</v>
@@ -8218,7 +8288,7 @@
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B26">
         <v>1</v>
@@ -8262,7 +8332,7 @@
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B27">
         <v>1</v>
@@ -8306,7 +8376,7 @@
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B28">
         <v>1</v>
@@ -8350,7 +8420,7 @@
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B29">
         <v>1</v>
@@ -8394,7 +8464,7 @@
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B30">
         <v>1</v>
@@ -8438,7 +8508,7 @@
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B31">
         <v>1</v>
@@ -8482,7 +8552,7 @@
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B32">
         <v>1</v>
@@ -8526,7 +8596,7 @@
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B33">
         <v>1</v>
@@ -8570,7 +8640,7 @@
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B34">
         <v>1</v>
@@ -8614,7 +8684,7 @@
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B35">
         <v>1</v>
@@ -8658,7 +8728,7 @@
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B36">
         <v>1</v>
@@ -8702,7 +8772,7 @@
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B37">
         <v>1</v>

</xml_diff>

<commit_message>
debugged constructing full sentence with template
</commit_message>
<xml_diff>
--- a/CDSData/CDS_SPARSE_2020_2021.xlsx
+++ b/CDSData/CDS_SPARSE_2020_2021.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhengy6\Desktop\rhit_IRPA_2023\CDSData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B6F5CAE-7538-43D3-9BCE-397D5FC4B031}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD4B5D82-9E38-4F32-B9FE-4968586C83C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="enrollment_general" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="719" uniqueCount="346">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="719" uniqueCount="348">
   <si>
     <t>Value</t>
   </si>
@@ -144,9 +144,6 @@
   </si>
   <si>
     <t>nan</t>
-  </si>
-  <si>
-    <t>The [aggregation] of [gender] [is_first_time] [is_first_year] [undergraduate_grade_level] [degree-goal] [student_level] enrolled is &lt;value&gt;</t>
   </si>
   <si>
     <t>Yes</t>
@@ -1075,6 +1072,15 @@
   </si>
   <si>
     <t>american indian</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>The [aggregation] of [gender] [is_first_time] [is_first_year] [undergraduate_grade_level] [degree-goal] [student_level] students enrolled is &lt;value&gt;</t>
+  </si>
+  <si>
+    <t>The (xor [aggregation] number) of [gender] [is_first_time] [is_first_year] [undergraduate_grade_level] [degree-goal] [student_level] students enrolled is &lt;value&gt;</t>
   </si>
 </sst>
 </file>
@@ -1423,9 +1429,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:W35"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="118.77734375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
@@ -3559,7 +3570,7 @@
     </row>
     <row r="31" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>36</v>
+        <v>347</v>
       </c>
       <c r="B31">
         <v>0</v>
@@ -3630,7 +3641,7 @@
     </row>
     <row r="32" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B32">
         <v>0</v>
@@ -3701,7 +3712,7 @@
     </row>
     <row r="33" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B33">
         <v>0</v>
@@ -3772,7 +3783,7 @@
     </row>
     <row r="34" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B34">
         <v>0</v>
@@ -3843,7 +3854,7 @@
     </row>
     <row r="35" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B35">
         <v>0</v>
@@ -3930,46 +3941,46 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>217</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>218</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>33</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="P1" s="1" t="s">
         <v>17</v>
@@ -3992,7 +4003,7 @@
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -4057,7 +4068,7 @@
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -4122,7 +4133,7 @@
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -4187,7 +4198,7 @@
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -4252,7 +4263,7 @@
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -4317,7 +4328,7 @@
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -4512,7 +4523,7 @@
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -4577,7 +4588,7 @@
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -4642,7 +4653,7 @@
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -4707,7 +4718,7 @@
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -4788,49 +4799,49 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>217</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>218</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>33</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>17</v>
@@ -4853,7 +4864,7 @@
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -4921,7 +4932,7 @@
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -4989,7 +5000,7 @@
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -5057,7 +5068,7 @@
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -5125,7 +5136,7 @@
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -5193,7 +5204,7 @@
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -5261,7 +5272,7 @@
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -5329,7 +5340,7 @@
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -5397,7 +5408,7 @@
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -5465,7 +5476,7 @@
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -5533,7 +5544,7 @@
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -5601,7 +5612,7 @@
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -5805,7 +5816,7 @@
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -5873,7 +5884,7 @@
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -5941,7 +5952,7 @@
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B18">
         <v>0</v>
@@ -6009,7 +6020,7 @@
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B19">
         <v>0</v>
@@ -6093,61 +6104,61 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="R1" s="1" t="s">
-        <v>244</v>
-      </c>
       <c r="S1" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="U1" s="1" t="s">
         <v>17</v>
@@ -6170,7 +6181,7 @@
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -6250,7 +6261,7 @@
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -6330,7 +6341,7 @@
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -6410,7 +6421,7 @@
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -6490,7 +6501,7 @@
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -6570,7 +6581,7 @@
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -6650,7 +6661,7 @@
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -6730,7 +6741,7 @@
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -6810,7 +6821,7 @@
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -6890,7 +6901,7 @@
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -6970,7 +6981,7 @@
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -7210,7 +7221,7 @@
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -7290,7 +7301,7 @@
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -7370,7 +7381,7 @@
     </row>
     <row r="17" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -7450,7 +7461,7 @@
     </row>
     <row r="18" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B18">
         <v>0</v>
@@ -7546,28 +7557,28 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>257</v>
-      </c>
       <c r="H1" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>17</v>
@@ -7590,7 +7601,7 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -7637,7 +7648,7 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -7684,7 +7695,7 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -7731,7 +7742,7 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -7778,7 +7789,7 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -7825,7 +7836,7 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -7966,7 +7977,7 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -8013,7 +8024,7 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -8060,7 +8071,7 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -8107,7 +8118,7 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -8180,67 +8191,67 @@
         <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>266</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>267</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>270</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="P1" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="R1" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="U1" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="T1" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>274</v>
-      </c>
       <c r="V1" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="X1" s="1" t="s">
         <v>26</v>
@@ -8249,28 +8260,28 @@
         <v>1</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="AA1" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="AB1" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>276</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>277</v>
       </c>
       <c r="AD1" s="1" t="s">
         <v>28</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AF1" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="AG1" s="1" t="s">
         <v>278</v>
-      </c>
-      <c r="AG1" s="1" t="s">
-        <v>279</v>
       </c>
       <c r="AH1" s="1" t="s">
         <v>17</v>
@@ -8290,7 +8301,7 @@
     </row>
     <row r="2" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -8406,7 +8417,7 @@
     </row>
     <row r="3" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -8522,7 +8533,7 @@
     </row>
     <row r="4" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -8638,7 +8649,7 @@
     </row>
     <row r="5" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -8754,7 +8765,7 @@
     </row>
     <row r="6" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -8870,7 +8881,7 @@
     </row>
     <row r="7" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -8986,7 +8997,7 @@
     </row>
     <row r="8" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -9102,7 +9113,7 @@
     </row>
     <row r="9" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -9218,7 +9229,7 @@
     </row>
     <row r="10" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -9334,7 +9345,7 @@
     </row>
     <row r="11" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -9450,7 +9461,7 @@
     </row>
     <row r="12" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -9566,7 +9577,7 @@
     </row>
     <row r="13" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -9682,7 +9693,7 @@
     </row>
     <row r="14" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -9798,7 +9809,7 @@
     </row>
     <row r="15" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -9914,7 +9925,7 @@
     </row>
     <row r="16" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -10030,7 +10041,7 @@
     </row>
     <row r="17" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -10146,7 +10157,7 @@
     </row>
     <row r="18" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B18">
         <v>0</v>
@@ -10262,7 +10273,7 @@
     </row>
     <row r="19" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B19">
         <v>0</v>
@@ -10378,7 +10389,7 @@
     </row>
     <row r="20" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B20">
         <v>0</v>
@@ -10494,7 +10505,7 @@
     </row>
     <row r="21" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B21">
         <v>0</v>
@@ -10610,7 +10621,7 @@
     </row>
     <row r="22" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B22">
         <v>0</v>
@@ -10842,7 +10853,7 @@
     </row>
     <row r="24" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B24">
         <v>0</v>
@@ -10958,7 +10969,7 @@
     </row>
     <row r="25" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B25">
         <v>0</v>
@@ -11074,7 +11085,7 @@
     </row>
     <row r="26" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B26">
         <v>0</v>
@@ -11190,7 +11201,7 @@
     </row>
     <row r="27" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B27">
         <v>0</v>
@@ -11325,10 +11336,10 @@
         <v>5</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>7</v>
@@ -11357,7 +11368,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -11395,7 +11406,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -11471,7 +11482,7 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -11509,7 +11520,7 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -11661,7 +11672,7 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -11699,7 +11710,7 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -11737,7 +11748,7 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -11775,7 +11786,7 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -11831,7 +11842,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -11852,61 +11863,61 @@
         <v>4</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>304</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>305</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>308</v>
       </c>
-      <c r="P1" s="1" t="s">
-        <v>272</v>
-      </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>309</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>310</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>311</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>312</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>313</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>314</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>315</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="Z1" s="1" t="s">
         <v>316</v>
       </c>
-      <c r="Y1" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>317</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>318</v>
       </c>
       <c r="AB1" s="1" t="s">
         <v>17</v>
@@ -11926,7 +11937,7 @@
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -12024,7 +12035,7 @@
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -12122,7 +12133,7 @@
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -12220,7 +12231,7 @@
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -12318,7 +12329,7 @@
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -12416,7 +12427,7 @@
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -12514,7 +12525,7 @@
     </row>
     <row r="8" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -12612,7 +12623,7 @@
     </row>
     <row r="9" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -12710,7 +12721,7 @@
     </row>
     <row r="10" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -12808,7 +12819,7 @@
     </row>
     <row r="11" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -12906,7 +12917,7 @@
     </row>
     <row r="12" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -13004,7 +13015,7 @@
     </row>
     <row r="13" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -13102,7 +13113,7 @@
     </row>
     <row r="14" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -13200,7 +13211,7 @@
     </row>
     <row r="15" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -13298,7 +13309,7 @@
     </row>
     <row r="16" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -13396,7 +13407,7 @@
     </row>
     <row r="17" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -13592,7 +13603,7 @@
     </row>
     <row r="19" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B19">
         <v>0</v>
@@ -13690,7 +13701,7 @@
     </row>
     <row r="20" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B20">
         <v>0</v>
@@ -13788,7 +13799,7 @@
     </row>
     <row r="21" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B21">
         <v>0</v>
@@ -13886,7 +13897,7 @@
     </row>
     <row r="22" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B22">
         <v>0</v>
@@ -14002,40 +14013,40 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>334</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>336</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>337</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>308</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>338</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>272</v>
-      </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>309</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>310</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>17</v>
@@ -14055,7 +14066,7 @@
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -14111,7 +14122,7 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -14167,7 +14178,7 @@
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -14223,7 +14234,7 @@
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -14279,7 +14290,7 @@
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -14391,7 +14402,7 @@
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -14447,7 +14458,7 @@
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -14503,7 +14514,7 @@
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -14559,7 +14570,7 @@
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -14622,11 +14633,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:W17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="79" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
@@ -14642,40 +14656,40 @@
         <v>7</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="H1" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>344</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>345</v>
-      </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>46</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>28</v>
       </c>
       <c r="O1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>48</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>17</v>
@@ -14696,12 +14710,12 @@
         <v>22</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -14772,7 +14786,7 @@
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -14843,7 +14857,7 @@
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -14914,7 +14928,7 @@
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -15056,7 +15070,7 @@
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -15198,7 +15212,7 @@
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -15269,7 +15283,7 @@
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -15411,7 +15425,7 @@
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>35</v>
+        <v>346</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -15482,7 +15496,7 @@
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -15553,7 +15567,7 @@
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -15624,7 +15638,7 @@
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -15695,7 +15709,7 @@
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -15766,7 +15780,7 @@
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>57</v>
+        <v>345</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -15873,40 +15887,40 @@
         <v>7</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>46</v>
       </c>
       <c r="P1" s="1" t="s">
         <v>28</v>
       </c>
       <c r="Q1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="R1" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>48</v>
       </c>
       <c r="S1" s="1" t="s">
         <v>17</v>
@@ -15927,12 +15941,12 @@
         <v>22</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -16009,7 +16023,7 @@
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -16086,7 +16100,7 @@
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -16163,7 +16177,7 @@
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -16317,7 +16331,7 @@
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -16471,7 +16485,7 @@
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -16779,7 +16793,7 @@
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -16856,7 +16870,7 @@
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -16933,7 +16947,7 @@
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -17010,7 +17024,7 @@
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -17087,7 +17101,7 @@
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -17186,79 +17200,79 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>78</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>79</v>
       </c>
       <c r="S1" s="2" t="s">
         <v>34</v>
       </c>
       <c r="T1" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="U1" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="X1" s="2" t="s">
         <v>83</v>
-      </c>
-      <c r="X1" s="2" t="s">
-        <v>84</v>
       </c>
       <c r="Y1" s="2" t="s">
         <v>33</v>
       </c>
       <c r="Z1" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="AA1" s="2" t="s">
         <v>17</v>
@@ -17281,7 +17295,7 @@
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B2" s="3">
         <v>1</v>
@@ -17379,7 +17393,7 @@
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B3" s="3">
         <v>1</v>
@@ -17477,7 +17491,7 @@
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B4" s="3">
         <v>1</v>
@@ -17869,7 +17883,7 @@
     </row>
     <row r="8" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B8" s="3">
         <v>0</v>
@@ -17967,7 +17981,7 @@
     </row>
     <row r="9" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B9" s="3">
         <v>0</v>
@@ -18065,7 +18079,7 @@
     </row>
     <row r="10" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B10" s="3">
         <v>0</v>
@@ -18163,7 +18177,7 @@
     </row>
     <row r="11" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B11" s="3">
         <v>1</v>
@@ -18261,7 +18275,7 @@
     </row>
     <row r="12" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B12" s="3">
         <v>1</v>
@@ -18359,7 +18373,7 @@
     </row>
     <row r="13" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B13" s="3">
         <v>1</v>
@@ -18457,7 +18471,7 @@
     </row>
     <row r="14" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B14" s="3">
         <v>1</v>
@@ -18653,7 +18667,7 @@
     </row>
     <row r="16" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B16" s="3">
         <v>1</v>
@@ -19045,7 +19059,7 @@
     </row>
     <row r="20" spans="1:32" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B20" s="3">
         <v>0</v>
@@ -19143,7 +19157,7 @@
     </row>
     <row r="21" spans="1:32" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B21" s="3">
         <v>0</v>
@@ -19241,7 +19255,7 @@
     </row>
     <row r="22" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B22" s="3">
         <v>0</v>
@@ -19339,7 +19353,7 @@
     </row>
     <row r="23" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B23" s="3">
         <v>0</v>
@@ -19437,7 +19451,7 @@
     </row>
     <row r="24" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B24" s="3">
         <v>0</v>
@@ -19535,7 +19549,7 @@
     </row>
     <row r="25" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B25" s="3">
         <v>0</v>
@@ -19650,61 +19664,61 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="R1" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="Q1" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>113</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>114</v>
       </c>
       <c r="U1" s="1" t="s">
         <v>17</v>
@@ -19712,7 +19726,7 @@
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -19777,7 +19791,7 @@
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -19842,7 +19856,7 @@
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -19907,7 +19921,7 @@
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -19972,7 +19986,7 @@
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -20037,7 +20051,7 @@
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -20102,7 +20116,7 @@
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -20167,7 +20181,7 @@
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -20232,7 +20246,7 @@
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -20297,7 +20311,7 @@
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -20362,7 +20376,7 @@
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -20427,7 +20441,7 @@
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -20492,7 +20506,7 @@
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -20557,7 +20571,7 @@
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -20622,7 +20636,7 @@
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -20687,7 +20701,7 @@
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -20752,7 +20766,7 @@
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B18">
         <v>0</v>
@@ -20817,7 +20831,7 @@
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B19">
         <v>0</v>
@@ -20882,7 +20896,7 @@
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B20">
         <v>0</v>
@@ -20947,7 +20961,7 @@
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B21">
         <v>0</v>
@@ -21028,69 +21042,69 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>140</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -21155,7 +21169,7 @@
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -21220,7 +21234,7 @@
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -21285,7 +21299,7 @@
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -21350,7 +21364,7 @@
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -21415,7 +21429,7 @@
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -21480,7 +21494,7 @@
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -21545,7 +21559,7 @@
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -21610,7 +21624,7 @@
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -21675,7 +21689,7 @@
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -21740,7 +21754,7 @@
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -21821,46 +21835,46 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>164</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>165</v>
       </c>
       <c r="P1" s="1" t="s">
         <v>17</v>
@@ -21883,7 +21897,7 @@
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -21948,7 +21962,7 @@
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -22013,7 +22027,7 @@
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -22078,7 +22092,7 @@
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -22143,7 +22157,7 @@
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -22208,7 +22222,7 @@
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -22273,7 +22287,7 @@
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -22338,7 +22352,7 @@
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -22403,7 +22417,7 @@
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -22468,7 +22482,7 @@
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -22533,7 +22547,7 @@
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -22598,7 +22612,7 @@
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -22663,7 +22677,7 @@
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -22728,7 +22742,7 @@
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -22793,7 +22807,7 @@
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -22858,7 +22872,7 @@
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -22923,7 +22937,7 @@
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B18">
         <v>0</v>
@@ -22988,7 +23002,7 @@
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B19">
         <v>0</v>
@@ -23053,7 +23067,7 @@
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B20">
         <v>0</v>
@@ -23118,7 +23132,7 @@
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B21">
         <v>0</v>
@@ -23183,7 +23197,7 @@
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B22">
         <v>0</v>
@@ -23248,7 +23262,7 @@
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B23">
         <v>0</v>
@@ -23313,7 +23327,7 @@
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B24">
         <v>0</v>
@@ -23378,7 +23392,7 @@
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B25">
         <v>0</v>
@@ -23443,7 +23457,7 @@
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B26">
         <v>0</v>
@@ -23508,7 +23522,7 @@
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B27">
         <v>0</v>
@@ -23573,7 +23587,7 @@
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B28">
         <v>0</v>
@@ -23638,7 +23652,7 @@
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B29">
         <v>0</v>
@@ -23703,7 +23717,7 @@
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B30">
         <v>0</v>
@@ -23768,7 +23782,7 @@
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B31">
         <v>0</v>
@@ -23833,7 +23847,7 @@
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B32">
         <v>0</v>
@@ -23898,7 +23912,7 @@
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B33">
         <v>0</v>
@@ -23963,7 +23977,7 @@
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B34">
         <v>0</v>
@@ -24028,7 +24042,7 @@
     </row>
     <row r="35" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B35">
         <v>0</v>
@@ -24093,7 +24107,7 @@
     </row>
     <row r="36" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B36">
         <v>0</v>
@@ -24158,7 +24172,7 @@
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B37">
         <v>0</v>
@@ -24353,7 +24367,7 @@
     </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B40">
         <v>0</v>
@@ -24418,7 +24432,7 @@
     </row>
     <row r="41" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B41">
         <v>0</v>
@@ -24483,7 +24497,7 @@
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B42">
         <v>0</v>
@@ -24548,7 +24562,7 @@
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B43">
         <v>0</v>
@@ -24629,52 +24643,52 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>197</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>198</v>
       </c>
       <c r="R1" s="1" t="s">
         <v>17</v>
@@ -24697,7 +24711,7 @@
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -24768,7 +24782,7 @@
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -24839,7 +24853,7 @@
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -24910,7 +24924,7 @@
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -24981,7 +24995,7 @@
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -25052,7 +25066,7 @@
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -25265,7 +25279,7 @@
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -25336,7 +25350,7 @@
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -25407,7 +25421,7 @@
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -25478,7 +25492,7 @@
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -25567,58 +25581,58 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>160</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="R1" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>88</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>89</v>
       </c>
       <c r="T1" s="1" t="s">
         <v>17</v>
@@ -25641,7 +25655,7 @@
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -25718,7 +25732,7 @@
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -25795,7 +25809,7 @@
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -25872,7 +25886,7 @@
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -25949,7 +25963,7 @@
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -26026,7 +26040,7 @@
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -26103,7 +26117,7 @@
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -26180,7 +26194,7 @@
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -26257,7 +26271,7 @@
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -26334,7 +26348,7 @@
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -26411,7 +26425,7 @@
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -26488,7 +26502,7 @@
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -26719,7 +26733,7 @@
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -26796,7 +26810,7 @@
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -26873,7 +26887,7 @@
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B18">
         <v>0</v>
@@ -26950,7 +26964,7 @@
     </row>
     <row r="19" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B19">
         <v>0</v>

</xml_diff>

<commit_message>
changed aggregate discrete range and fixed some more bugs
</commit_message>
<xml_diff>
--- a/CDSData/CDS_SPARSE_2020_2021.xlsx
+++ b/CDSData/CDS_SPARSE_2020_2021.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhengy6\Desktop\rhit_IRPA_2023\CDSData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD4B5D82-9E38-4F32-B9FE-4968586C83C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{773A52CD-4097-4527-8600-70752B63A24B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="9" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="enrollment_general" sheetId="2" r:id="rId1"/>
@@ -1429,8 +1429,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:W35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4790,9 +4790,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:V19"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="8" max="8" width="8.88671875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
@@ -6095,7 +6100,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:Z18"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -24634,9 +24641,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:W13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="21" max="21" width="27.6640625" customWidth="1"/>
+    <col min="22" max="22" width="33.88671875" customWidth="1"/>
+    <col min="23" max="23" width="33.109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
@@ -25350,7 +25364,7 @@
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -25571,10 +25585,13 @@
   <dimension ref="A1:Y19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M26" sqref="M26"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="9" max="9" width="12.5546875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">

</xml_diff>